<commit_message>
corrected errors in metabolite names
</commit_message>
<xml_diff>
--- a/Data/Opening_reactions2.xlsx
+++ b/Data/Opening_reactions2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonyrainbow/cobradata1/Datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8AECD6-C5FD-8049-A184-525CE687C5F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F694DDF5-AACE-6F47-856E-47E4E5726665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="3680" windowWidth="27360" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5120" yWindow="2360" windowWidth="27360" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>EX_pchol_hs[e]</t>
   </si>
@@ -60,9 +60,6 @@
     <t>EX_chsterol[e]</t>
   </si>
   <si>
-    <t>EX_clpn_hs[e]</t>
-  </si>
-  <si>
     <t>EX_pail_hs[e]</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>EX_ile_L[e]</t>
   </si>
   <si>
-    <t>EX_iso_L[e]</t>
-  </si>
-  <si>
     <t>EX_leu_L[e]</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>EX_pydxn[e]</t>
   </si>
   <si>
-    <t>EX_rbflv[e]</t>
-  </si>
-  <si>
     <t>EX_thm[e]</t>
   </si>
   <si>
@@ -174,9 +165,6 @@
     <t>EX_utp[e]</t>
   </si>
   <si>
-    <t>EX_g6p[e]</t>
-  </si>
-  <si>
     <t>EX_pyr[e]</t>
   </si>
   <si>
@@ -189,9 +177,6 @@
     <t>EX_co2[e]</t>
   </si>
   <si>
-    <t>EX_hco3[e</t>
-  </si>
-  <si>
     <t>EX_acetone[e]</t>
   </si>
   <si>
@@ -222,15 +207,9 @@
     <t>EX_urate[e]</t>
   </si>
   <si>
-    <t>EX_xolest[e]</t>
-  </si>
-  <si>
     <t>EX_ahdt[e]</t>
   </si>
   <si>
-    <t>EX_dtmpt[e]</t>
-  </si>
-  <si>
     <t>EX_dttp[e]</t>
   </si>
   <si>
@@ -280,6 +259,21 @@
   </si>
   <si>
     <t>EX_na1[e]</t>
+  </si>
+  <si>
+    <t>EX_xolest_hs[e]</t>
+  </si>
+  <si>
+    <t>EX_ribflv[e]</t>
+  </si>
+  <si>
+    <t>EX_hco3[e]</t>
+  </si>
+  <si>
+    <t>EX_clpnd_hs[e]</t>
+  </si>
+  <si>
+    <t>EX_dtmp[e]</t>
   </si>
 </sst>
 </file>
@@ -627,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="164" zoomScaleNormal="164" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="164" zoomScaleNormal="164" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,7 +635,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -652,7 +646,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -663,7 +657,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -674,7 +668,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -685,7 +679,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3">
         <v>-0.39810427999999998</v>
@@ -696,7 +690,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -707,7 +701,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -718,7 +712,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -740,7 +734,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -751,7 +745,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3">
         <v>-2.8571428999999999E-2</v>
@@ -773,7 +767,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -784,7 +778,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -795,7 +789,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -806,7 +800,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -817,7 +811,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>-0.20127796000000001</v>
@@ -828,7 +822,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -850,7 +844,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -861,7 +855,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
@@ -872,7 +866,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -883,7 +877,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -905,7 +899,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2">
         <v>-8.9999999999999993E-3</v>
@@ -916,10 +910,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="B26" s="2">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="C26" s="2">
         <v>1000</v>
@@ -927,10 +921,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B27" s="2">
-        <v>-25</v>
+        <v>-4</v>
       </c>
       <c r="C27" s="2">
         <v>1000</v>
@@ -941,7 +935,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="2">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="C28" s="2">
         <v>1000</v>
@@ -952,7 +946,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="2">
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="C29" s="2">
         <v>1000</v>
@@ -960,10 +954,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="B30" s="2">
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="C30" s="2">
         <v>1000</v>
@@ -971,7 +965,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2">
         <v>0</v>
@@ -982,7 +976,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
@@ -993,10 +987,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B33" s="2">
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="C33" s="2">
         <v>1000</v>
@@ -1004,10 +998,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B34" s="2">
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="C34" s="2">
         <v>1000</v>
@@ -1015,7 +1009,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
@@ -1026,7 +1020,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -1037,7 +1031,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B37" s="2">
         <v>0</v>
@@ -1048,10 +1042,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B38" s="2">
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="C38" s="2">
         <v>1000</v>
@@ -1059,10 +1053,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="B39" s="2">
-        <v>-1000</v>
+        <v>-0.2</v>
       </c>
       <c r="C39" s="2">
         <v>1000</v>
@@ -1070,10 +1064,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="B40" s="2">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="C40" s="2">
         <v>1000</v>
@@ -1081,10 +1075,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="2">
-        <v>-0.8</v>
+        <v>36</v>
+      </c>
+      <c r="B41" s="3">
+        <v>-0.04</v>
       </c>
       <c r="C41" s="2">
         <v>1000</v>
@@ -1092,10 +1086,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B42" s="2">
-        <v>0</v>
+        <v>-0.80152670000000004</v>
       </c>
       <c r="C42" s="2">
         <v>1000</v>
@@ -1103,10 +1097,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="3">
-        <v>-0.04</v>
+        <v>75</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0</v>
       </c>
       <c r="C43" s="2">
         <v>1000</v>
@@ -1114,9 +1108,9 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="2">
+        <v>24</v>
+      </c>
+      <c r="B44" s="3">
         <v>-0.80152670000000004</v>
       </c>
       <c r="C44" s="2">
@@ -1125,7 +1119,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B45" s="2">
         <v>0</v>
@@ -1136,10 +1130,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" s="3">
-        <v>-0.80152670000000004</v>
+        <v>-0.79781420000000003</v>
       </c>
       <c r="C46" s="2">
         <v>1000</v>
@@ -1147,10 +1141,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="2">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B47" s="3">
+        <v>-0.20134228000000001</v>
       </c>
       <c r="C47" s="2">
         <v>1000</v>
@@ -1158,10 +1152,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="B48" s="3">
-        <v>-0.79781420000000003</v>
+        <v>-1</v>
       </c>
       <c r="C48" s="2">
         <v>1000</v>
@@ -1169,10 +1163,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B49" s="3">
-        <v>-0.20134228000000001</v>
+        <v>-3.2786883000000003E-2</v>
       </c>
       <c r="C49" s="2">
         <v>1000</v>
@@ -1180,10 +1174,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="3">
-        <v>-1</v>
+        <v>68</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0</v>
       </c>
       <c r="C50" s="2">
         <v>1000</v>
@@ -1191,10 +1185,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B51" s="3">
-        <v>-3.2786883000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="C51" s="2">
         <v>1000</v>
@@ -1202,10 +1196,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="B52" s="2">
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="C52" s="2">
         <v>1000</v>
@@ -1213,9 +1207,9 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="3">
+        <v>55</v>
+      </c>
+      <c r="B53" s="2">
         <v>0</v>
       </c>
       <c r="C53" s="2">
@@ -1224,10 +1218,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B54" s="2">
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="C54" s="2">
         <v>1000</v>
@@ -1235,7 +1229,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="B55" s="2">
         <v>0</v>
@@ -1246,7 +1240,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B56" s="2">
         <v>0</v>
@@ -1257,7 +1251,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B57" s="2">
         <v>0</v>
@@ -1268,7 +1262,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B58" s="2">
         <v>0</v>
@@ -1279,7 +1273,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B59" s="2">
         <v>0</v>
@@ -1290,10 +1284,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="B60" s="2">
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="C60" s="2">
         <v>1000</v>
@@ -1301,10 +1295,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" s="2">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="B61" s="3">
+        <v>-8.3857440000000005E-3</v>
       </c>
       <c r="C61" s="2">
         <v>1000</v>
@@ -1312,10 +1306,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B62" s="2">
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="C62" s="2">
         <v>1000</v>
@@ -1323,10 +1317,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B63" s="3">
-        <v>-8.3857440000000005E-3</v>
+        <v>11</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0</v>
       </c>
       <c r="C63" s="2">
         <v>1000</v>
@@ -1334,10 +1328,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" s="2">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="B64" s="4">
+        <v>-1.9417475999999999E-2</v>
       </c>
       <c r="C64" s="2">
         <v>1000</v>
@@ -1345,10 +1339,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B65" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C65" s="2">
         <v>1000</v>
@@ -1356,10 +1350,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B66" s="4">
-        <v>-1.9417475999999999E-2</v>
+        <v>78</v>
+      </c>
+      <c r="B66" s="3">
+        <v>-1.0638297999999999E-3</v>
       </c>
       <c r="C66" s="2">
         <v>1000</v>
@@ -1367,10 +1361,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B67" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C67" s="2">
         <v>1000</v>
@@ -1378,10 +1372,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B68" s="3">
-        <v>-1.0638297999999999E-3</v>
+        <v>29</v>
+      </c>
+      <c r="B68" s="2">
+        <v>-0.4</v>
       </c>
       <c r="C68" s="2">
         <v>1000</v>
@@ -1389,7 +1383,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="B69" s="2">
         <v>0</v>
@@ -1400,10 +1394,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B70" s="2">
-        <v>-0.4</v>
+        <v>40</v>
+      </c>
+      <c r="B70" s="3">
+        <v>-1.1869436000000001E-2</v>
       </c>
       <c r="C70" s="2">
         <v>1000</v>
@@ -1411,7 +1405,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B71" s="2">
         <v>0</v>
@@ -1422,10 +1416,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B72" s="3">
-        <v>-1.1869436000000001E-2</v>
+        <v>-0.79831934000000004</v>
       </c>
       <c r="C72" s="2">
         <v>1000</v>
@@ -1433,10 +1427,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B73" s="2">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="B73" s="3">
+        <v>-7.8431374999999998E-2</v>
       </c>
       <c r="C73" s="2">
         <v>1000</v>
@@ -1447,7 +1441,7 @@
         <v>32</v>
       </c>
       <c r="B74" s="3">
-        <v>-0.79831934000000004</v>
+        <v>-0.39779004000000001</v>
       </c>
       <c r="C74" s="2">
         <v>1000</v>
@@ -1455,10 +1449,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B75" s="3">
-        <v>-7.8431374999999998E-2</v>
+        <v>72</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0</v>
       </c>
       <c r="C75" s="2">
         <v>1000</v>
@@ -1466,10 +1460,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B76" s="3">
-        <v>-0.39779004000000001</v>
+        <v>58</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0</v>
       </c>
       <c r="C76" s="2">
         <v>1000</v>
@@ -1477,7 +1471,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B77" s="2">
         <v>0</v>
@@ -1488,10 +1482,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B78" s="2">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="B78" s="3">
+        <v>-0.80341879999999999</v>
       </c>
       <c r="C78" s="2">
         <v>1000</v>
@@ -1499,7 +1493,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B79" s="2">
         <v>0</v>
@@ -1510,40 +1504,18 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B80" s="3">
-        <v>-0.80341879999999999</v>
+        <v>71</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0</v>
       </c>
       <c r="C80" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B81" s="2">
-        <v>0</v>
-      </c>
-      <c r="C81" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B82" s="2">
-        <v>0</v>
-      </c>
-      <c r="C82" s="2">
-        <v>1000</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C85">
-    <sortCondition ref="A2:A85"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C83">
+    <sortCondition ref="A2:A83"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>